<commit_message>
update keyword table and test set
</commit_message>
<xml_diff>
--- a/keyword_table/xlsx/Table_RepKeyword_xlsx.xlsx
+++ b/keyword_table/xlsx/Table_RepKeyword_xlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="782">
   <si>
     <t>가상화 솔루션</t>
   </si>
@@ -909,9 +909,6 @@
   </si>
   <si>
     <t>IR</t>
-  </si>
-  <si>
-    <t>log</t>
   </si>
   <si>
     <t>json</t>
@@ -2705,20 +2702,20 @@
   <dimension ref="A1:C778"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B1" t="s">
         <v>780</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>781</v>
-      </c>
-      <c r="C1" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -6271,7 +6268,7 @@
         <v>323</v>
       </c>
       <c r="C324" t="s">
-        <v>1</v>
+        <v>324</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
@@ -6279,10 +6276,10 @@
         <v>324</v>
       </c>
       <c r="B325" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C325" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
@@ -6293,7 +6290,7 @@
         <v>326</v>
       </c>
       <c r="C326" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.3">
@@ -6304,7 +6301,7 @@
         <v>327</v>
       </c>
       <c r="C327" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
@@ -6315,7 +6312,7 @@
         <v>328</v>
       </c>
       <c r="C328" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
@@ -6326,7 +6323,7 @@
         <v>329</v>
       </c>
       <c r="C329" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
@@ -6337,7 +6334,7 @@
         <v>330</v>
       </c>
       <c r="C330" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.3">
@@ -6348,7 +6345,7 @@
         <v>331</v>
       </c>
       <c r="C331" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
@@ -6359,7 +6356,7 @@
         <v>332</v>
       </c>
       <c r="C332" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
@@ -6370,7 +6367,7 @@
         <v>333</v>
       </c>
       <c r="C333" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
@@ -6381,7 +6378,7 @@
         <v>334</v>
       </c>
       <c r="C334" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
@@ -6392,7 +6389,7 @@
         <v>335</v>
       </c>
       <c r="C335" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
@@ -6403,7 +6400,7 @@
         <v>336</v>
       </c>
       <c r="C336" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
@@ -6414,7 +6411,7 @@
         <v>337</v>
       </c>
       <c r="C337" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
@@ -6425,7 +6422,7 @@
         <v>338</v>
       </c>
       <c r="C338" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
@@ -6436,7 +6433,7 @@
         <v>339</v>
       </c>
       <c r="C339" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
@@ -6447,7 +6444,7 @@
         <v>340</v>
       </c>
       <c r="C340" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
@@ -6458,7 +6455,7 @@
         <v>341</v>
       </c>
       <c r="C341" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
@@ -6469,7 +6466,7 @@
         <v>342</v>
       </c>
       <c r="C342" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
@@ -6480,7 +6477,7 @@
         <v>343</v>
       </c>
       <c r="C343" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
@@ -6491,7 +6488,7 @@
         <v>344</v>
       </c>
       <c r="C344" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
@@ -6502,7 +6499,7 @@
         <v>345</v>
       </c>
       <c r="C345" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
@@ -6513,7 +6510,7 @@
         <v>346</v>
       </c>
       <c r="C346" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
@@ -6524,7 +6521,7 @@
         <v>347</v>
       </c>
       <c r="C347" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
@@ -6535,7 +6532,7 @@
         <v>348</v>
       </c>
       <c r="C348" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
@@ -6546,7 +6543,7 @@
         <v>349</v>
       </c>
       <c r="C349" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
@@ -6557,7 +6554,7 @@
         <v>350</v>
       </c>
       <c r="C350" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
@@ -6568,7 +6565,7 @@
         <v>351</v>
       </c>
       <c r="C351" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
@@ -6579,7 +6576,7 @@
         <v>352</v>
       </c>
       <c r="C352" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
@@ -6590,7 +6587,7 @@
         <v>353</v>
       </c>
       <c r="C353" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
@@ -6601,7 +6598,7 @@
         <v>354</v>
       </c>
       <c r="C354" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
@@ -6612,7 +6609,7 @@
         <v>355</v>
       </c>
       <c r="C355" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.3">
@@ -6623,7 +6620,7 @@
         <v>356</v>
       </c>
       <c r="C356" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
@@ -6634,7 +6631,7 @@
         <v>357</v>
       </c>
       <c r="C357" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
@@ -6645,7 +6642,7 @@
         <v>358</v>
       </c>
       <c r="C358" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.3">
@@ -6656,7 +6653,7 @@
         <v>359</v>
       </c>
       <c r="C359" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.3">
@@ -6667,7 +6664,7 @@
         <v>360</v>
       </c>
       <c r="C360" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.3">
@@ -6678,7 +6675,7 @@
         <v>361</v>
       </c>
       <c r="C361" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
@@ -6689,7 +6686,7 @@
         <v>362</v>
       </c>
       <c r="C362" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
@@ -6700,7 +6697,7 @@
         <v>363</v>
       </c>
       <c r="C363" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
@@ -6711,7 +6708,7 @@
         <v>364</v>
       </c>
       <c r="C364" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
@@ -6722,7 +6719,7 @@
         <v>365</v>
       </c>
       <c r="C365" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
@@ -6733,7 +6730,7 @@
         <v>366</v>
       </c>
       <c r="C366" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.3">
@@ -6744,7 +6741,7 @@
         <v>367</v>
       </c>
       <c r="C367" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
@@ -6755,7 +6752,7 @@
         <v>368</v>
       </c>
       <c r="C368" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
@@ -6766,7 +6763,7 @@
         <v>369</v>
       </c>
       <c r="C369" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
@@ -6777,7 +6774,7 @@
         <v>370</v>
       </c>
       <c r="C370" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
@@ -6788,7 +6785,7 @@
         <v>371</v>
       </c>
       <c r="C371" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
@@ -6799,7 +6796,7 @@
         <v>372</v>
       </c>
       <c r="C372" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
@@ -6810,7 +6807,7 @@
         <v>373</v>
       </c>
       <c r="C373" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
@@ -6821,7 +6818,7 @@
         <v>374</v>
       </c>
       <c r="C374" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
@@ -6832,7 +6829,7 @@
         <v>375</v>
       </c>
       <c r="C375" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
@@ -6843,7 +6840,7 @@
         <v>376</v>
       </c>
       <c r="C376" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
@@ -6854,7 +6851,7 @@
         <v>377</v>
       </c>
       <c r="C377" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
@@ -6865,7 +6862,7 @@
         <v>378</v>
       </c>
       <c r="C378" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
@@ -6876,7 +6873,7 @@
         <v>379</v>
       </c>
       <c r="C379" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
@@ -6887,7 +6884,7 @@
         <v>380</v>
       </c>
       <c r="C380" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
@@ -6898,7 +6895,7 @@
         <v>381</v>
       </c>
       <c r="C381" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
@@ -6909,7 +6906,7 @@
         <v>382</v>
       </c>
       <c r="C382" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
@@ -6920,7 +6917,7 @@
         <v>383</v>
       </c>
       <c r="C383" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
@@ -6931,7 +6928,7 @@
         <v>384</v>
       </c>
       <c r="C384" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
@@ -6942,7 +6939,7 @@
         <v>385</v>
       </c>
       <c r="C385" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
@@ -6953,7 +6950,7 @@
         <v>386</v>
       </c>
       <c r="C386" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
@@ -6964,7 +6961,7 @@
         <v>387</v>
       </c>
       <c r="C387" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.3">
@@ -6975,7 +6972,7 @@
         <v>388</v>
       </c>
       <c r="C388" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
@@ -6986,7 +6983,7 @@
         <v>389</v>
       </c>
       <c r="C389" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
@@ -6997,7 +6994,7 @@
         <v>390</v>
       </c>
       <c r="C390" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
@@ -7008,7 +7005,7 @@
         <v>391</v>
       </c>
       <c r="C391" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
@@ -7019,7 +7016,7 @@
         <v>392</v>
       </c>
       <c r="C392" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
@@ -7030,7 +7027,7 @@
         <v>393</v>
       </c>
       <c r="C393" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
@@ -7041,7 +7038,7 @@
         <v>394</v>
       </c>
       <c r="C394" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
@@ -7052,7 +7049,7 @@
         <v>395</v>
       </c>
       <c r="C395" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
@@ -7063,7 +7060,7 @@
         <v>396</v>
       </c>
       <c r="C396" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
@@ -7074,7 +7071,7 @@
         <v>397</v>
       </c>
       <c r="C397" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
@@ -7085,7 +7082,7 @@
         <v>398</v>
       </c>
       <c r="C398" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.3">
@@ -7096,7 +7093,7 @@
         <v>399</v>
       </c>
       <c r="C399" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.3">
@@ -7107,7 +7104,7 @@
         <v>400</v>
       </c>
       <c r="C400" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.3">
@@ -7118,7 +7115,7 @@
         <v>401</v>
       </c>
       <c r="C401" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
@@ -7129,7 +7126,7 @@
         <v>402</v>
       </c>
       <c r="C402" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.3">
@@ -7140,7 +7137,7 @@
         <v>403</v>
       </c>
       <c r="C403" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.3">
@@ -7151,7 +7148,7 @@
         <v>404</v>
       </c>
       <c r="C404" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.3">
@@ -7162,7 +7159,7 @@
         <v>405</v>
       </c>
       <c r="C405" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.3">
@@ -7173,7 +7170,7 @@
         <v>406</v>
       </c>
       <c r="C406" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.3">
@@ -7184,7 +7181,7 @@
         <v>407</v>
       </c>
       <c r="C407" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.3">
@@ -7195,7 +7192,7 @@
         <v>408</v>
       </c>
       <c r="C408" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.3">
@@ -7206,7 +7203,7 @@
         <v>409</v>
       </c>
       <c r="C409" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.3">
@@ -7217,7 +7214,7 @@
         <v>410</v>
       </c>
       <c r="C410" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.3">
@@ -7228,7 +7225,7 @@
         <v>411</v>
       </c>
       <c r="C411" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.3">
@@ -7239,7 +7236,7 @@
         <v>412</v>
       </c>
       <c r="C412" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.3">
@@ -7250,7 +7247,7 @@
         <v>413</v>
       </c>
       <c r="C413" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.3">
@@ -7261,7 +7258,7 @@
         <v>414</v>
       </c>
       <c r="C414" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
@@ -7272,7 +7269,7 @@
         <v>415</v>
       </c>
       <c r="C415" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
@@ -7283,7 +7280,7 @@
         <v>416</v>
       </c>
       <c r="C416" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.3">
@@ -7294,7 +7291,7 @@
         <v>417</v>
       </c>
       <c r="C417" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.3">
@@ -7305,7 +7302,7 @@
         <v>418</v>
       </c>
       <c r="C418" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.3">
@@ -7316,7 +7313,7 @@
         <v>419</v>
       </c>
       <c r="C419" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
@@ -7327,7 +7324,7 @@
         <v>420</v>
       </c>
       <c r="C420" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
@@ -7338,7 +7335,7 @@
         <v>421</v>
       </c>
       <c r="C421" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.3">
@@ -7349,7 +7346,7 @@
         <v>422</v>
       </c>
       <c r="C422" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.3">
@@ -7360,7 +7357,7 @@
         <v>423</v>
       </c>
       <c r="C423" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.3">
@@ -7371,7 +7368,7 @@
         <v>424</v>
       </c>
       <c r="C424" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.3">
@@ -7382,7 +7379,7 @@
         <v>425</v>
       </c>
       <c r="C425" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.3">
@@ -7393,7 +7390,7 @@
         <v>426</v>
       </c>
       <c r="C426" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.3">
@@ -7404,7 +7401,7 @@
         <v>427</v>
       </c>
       <c r="C427" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.3">
@@ -7415,7 +7412,7 @@
         <v>428</v>
       </c>
       <c r="C428" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.3">
@@ -7426,7 +7423,7 @@
         <v>429</v>
       </c>
       <c r="C429" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.3">
@@ -7437,7 +7434,7 @@
         <v>430</v>
       </c>
       <c r="C430" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.3">
@@ -7448,7 +7445,7 @@
         <v>431</v>
       </c>
       <c r="C431" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.3">
@@ -7459,7 +7456,7 @@
         <v>432</v>
       </c>
       <c r="C432" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.3">
@@ -7470,7 +7467,7 @@
         <v>433</v>
       </c>
       <c r="C433" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.3">
@@ -7481,7 +7478,7 @@
         <v>434</v>
       </c>
       <c r="C434" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.3">
@@ -7492,7 +7489,7 @@
         <v>435</v>
       </c>
       <c r="C435" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.3">
@@ -7503,7 +7500,7 @@
         <v>436</v>
       </c>
       <c r="C436" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.3">
@@ -7514,7 +7511,7 @@
         <v>437</v>
       </c>
       <c r="C437" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.3">
@@ -7525,7 +7522,7 @@
         <v>438</v>
       </c>
       <c r="C438" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.3">
@@ -7536,7 +7533,7 @@
         <v>439</v>
       </c>
       <c r="C439" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.3">
@@ -7547,7 +7544,7 @@
         <v>440</v>
       </c>
       <c r="C440" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.3">
@@ -7558,7 +7555,7 @@
         <v>441</v>
       </c>
       <c r="C441" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.3">
@@ -7569,7 +7566,7 @@
         <v>442</v>
       </c>
       <c r="C442" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.3">
@@ -7580,7 +7577,7 @@
         <v>443</v>
       </c>
       <c r="C443" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.3">
@@ -7591,7 +7588,7 @@
         <v>444</v>
       </c>
       <c r="C444" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.3">
@@ -7602,7 +7599,7 @@
         <v>445</v>
       </c>
       <c r="C445" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.3">
@@ -7613,7 +7610,7 @@
         <v>446</v>
       </c>
       <c r="C446" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.3">
@@ -7624,7 +7621,7 @@
         <v>447</v>
       </c>
       <c r="C447" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.3">
@@ -7635,7 +7632,7 @@
         <v>448</v>
       </c>
       <c r="C448" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.3">
@@ -7646,7 +7643,7 @@
         <v>449</v>
       </c>
       <c r="C449" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.3">
@@ -7657,7 +7654,7 @@
         <v>450</v>
       </c>
       <c r="C450" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.3">
@@ -7668,7 +7665,7 @@
         <v>451</v>
       </c>
       <c r="C451" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.3">
@@ -7679,7 +7676,7 @@
         <v>452</v>
       </c>
       <c r="C452" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.3">
@@ -7690,7 +7687,7 @@
         <v>453</v>
       </c>
       <c r="C453" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.3">
@@ -7701,7 +7698,7 @@
         <v>454</v>
       </c>
       <c r="C454" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.3">
@@ -7712,7 +7709,7 @@
         <v>455</v>
       </c>
       <c r="C455" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.3">
@@ -7723,7 +7720,7 @@
         <v>456</v>
       </c>
       <c r="C456" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.3">
@@ -7734,7 +7731,7 @@
         <v>457</v>
       </c>
       <c r="C457" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.3">
@@ -7745,7 +7742,7 @@
         <v>458</v>
       </c>
       <c r="C458" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.3">
@@ -7756,7 +7753,7 @@
         <v>459</v>
       </c>
       <c r="C459" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.3">
@@ -7767,7 +7764,7 @@
         <v>460</v>
       </c>
       <c r="C460" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.3">
@@ -7778,7 +7775,7 @@
         <v>461</v>
       </c>
       <c r="C461" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.3">
@@ -7789,7 +7786,7 @@
         <v>462</v>
       </c>
       <c r="C462" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.3">
@@ -7800,7 +7797,7 @@
         <v>463</v>
       </c>
       <c r="C463" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.3">
@@ -7811,7 +7808,7 @@
         <v>464</v>
       </c>
       <c r="C464" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.3">
@@ -7822,7 +7819,7 @@
         <v>465</v>
       </c>
       <c r="C465" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.3">
@@ -7833,7 +7830,7 @@
         <v>466</v>
       </c>
       <c r="C466" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.3">
@@ -7844,7 +7841,7 @@
         <v>467</v>
       </c>
       <c r="C467" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.3">
@@ -7855,7 +7852,7 @@
         <v>468</v>
       </c>
       <c r="C468" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.3">
@@ -7866,7 +7863,7 @@
         <v>469</v>
       </c>
       <c r="C469" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.3">
@@ -7877,7 +7874,7 @@
         <v>470</v>
       </c>
       <c r="C470" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.3">
@@ -7888,7 +7885,7 @@
         <v>471</v>
       </c>
       <c r="C471" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.3">
@@ -7899,7 +7896,7 @@
         <v>472</v>
       </c>
       <c r="C472" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.3">
@@ -7910,7 +7907,7 @@
         <v>473</v>
       </c>
       <c r="C473" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.3">
@@ -7921,7 +7918,7 @@
         <v>474</v>
       </c>
       <c r="C474" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.3">
@@ -7932,7 +7929,7 @@
         <v>475</v>
       </c>
       <c r="C475" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.3">
@@ -7943,7 +7940,7 @@
         <v>476</v>
       </c>
       <c r="C476" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.3">
@@ -7954,7 +7951,7 @@
         <v>477</v>
       </c>
       <c r="C477" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.3">
@@ -7965,7 +7962,7 @@
         <v>478</v>
       </c>
       <c r="C478" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.3">
@@ -7976,7 +7973,7 @@
         <v>479</v>
       </c>
       <c r="C479" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.3">
@@ -7987,7 +7984,7 @@
         <v>480</v>
       </c>
       <c r="C480" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.3">
@@ -7998,7 +7995,7 @@
         <v>481</v>
       </c>
       <c r="C481" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.3">
@@ -8009,7 +8006,7 @@
         <v>482</v>
       </c>
       <c r="C482" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.3">
@@ -8020,7 +8017,7 @@
         <v>483</v>
       </c>
       <c r="C483" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.3">
@@ -8031,7 +8028,7 @@
         <v>484</v>
       </c>
       <c r="C484" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.3">
@@ -8042,7 +8039,7 @@
         <v>485</v>
       </c>
       <c r="C485" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.3">
@@ -8053,7 +8050,7 @@
         <v>486</v>
       </c>
       <c r="C486" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.3">
@@ -8064,7 +8061,7 @@
         <v>487</v>
       </c>
       <c r="C487" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.3">
@@ -8075,7 +8072,7 @@
         <v>488</v>
       </c>
       <c r="C488" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.3">
@@ -8086,7 +8083,7 @@
         <v>489</v>
       </c>
       <c r="C489" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.3">
@@ -8097,7 +8094,7 @@
         <v>490</v>
       </c>
       <c r="C490" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.3">
@@ -8108,7 +8105,7 @@
         <v>491</v>
       </c>
       <c r="C491" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.3">
@@ -8119,7 +8116,7 @@
         <v>492</v>
       </c>
       <c r="C492" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.3">
@@ -8130,7 +8127,7 @@
         <v>493</v>
       </c>
       <c r="C493" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.3">
@@ -8141,7 +8138,7 @@
         <v>494</v>
       </c>
       <c r="C494" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.3">
@@ -8152,7 +8149,7 @@
         <v>495</v>
       </c>
       <c r="C495" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.3">
@@ -8163,7 +8160,7 @@
         <v>496</v>
       </c>
       <c r="C496" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.3">
@@ -8174,7 +8171,7 @@
         <v>497</v>
       </c>
       <c r="C497" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.3">
@@ -8185,7 +8182,7 @@
         <v>498</v>
       </c>
       <c r="C498" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.3">
@@ -8196,7 +8193,7 @@
         <v>499</v>
       </c>
       <c r="C499" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.3">
@@ -8207,7 +8204,7 @@
         <v>500</v>
       </c>
       <c r="C500" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.3">
@@ -8218,7 +8215,7 @@
         <v>501</v>
       </c>
       <c r="C501" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.3">
@@ -8229,7 +8226,7 @@
         <v>502</v>
       </c>
       <c r="C502" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.3">
@@ -8240,7 +8237,7 @@
         <v>503</v>
       </c>
       <c r="C503" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.3">
@@ -8251,7 +8248,7 @@
         <v>504</v>
       </c>
       <c r="C504" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.3">
@@ -8262,7 +8259,7 @@
         <v>505</v>
       </c>
       <c r="C505" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.3">
@@ -8273,7 +8270,7 @@
         <v>506</v>
       </c>
       <c r="C506" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.3">
@@ -8284,7 +8281,7 @@
         <v>507</v>
       </c>
       <c r="C507" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.3">
@@ -8295,7 +8292,7 @@
         <v>508</v>
       </c>
       <c r="C508" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.3">
@@ -8306,7 +8303,7 @@
         <v>509</v>
       </c>
       <c r="C509" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.3">
@@ -8317,7 +8314,7 @@
         <v>510</v>
       </c>
       <c r="C510" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.3">
@@ -8328,7 +8325,7 @@
         <v>511</v>
       </c>
       <c r="C511" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.3">
@@ -8339,7 +8336,7 @@
         <v>512</v>
       </c>
       <c r="C512" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.3">
@@ -8350,7 +8347,7 @@
         <v>513</v>
       </c>
       <c r="C513" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.3">
@@ -8361,7 +8358,7 @@
         <v>514</v>
       </c>
       <c r="C514" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.3">
@@ -8372,7 +8369,7 @@
         <v>515</v>
       </c>
       <c r="C515" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.3">
@@ -8383,7 +8380,7 @@
         <v>516</v>
       </c>
       <c r="C516" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.3">
@@ -8394,7 +8391,7 @@
         <v>517</v>
       </c>
       <c r="C517" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.3">
@@ -8405,7 +8402,7 @@
         <v>518</v>
       </c>
       <c r="C518" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.3">
@@ -8416,7 +8413,7 @@
         <v>519</v>
       </c>
       <c r="C519" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.3">
@@ -8427,7 +8424,7 @@
         <v>520</v>
       </c>
       <c r="C520" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.3">
@@ -8438,7 +8435,7 @@
         <v>521</v>
       </c>
       <c r="C521" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.3">
@@ -8449,7 +8446,7 @@
         <v>522</v>
       </c>
       <c r="C522" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.3">
@@ -8460,7 +8457,7 @@
         <v>523</v>
       </c>
       <c r="C523" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.3">
@@ -8471,7 +8468,7 @@
         <v>524</v>
       </c>
       <c r="C524" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.3">
@@ -8482,7 +8479,7 @@
         <v>525</v>
       </c>
       <c r="C525" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.3">
@@ -8493,7 +8490,7 @@
         <v>526</v>
       </c>
       <c r="C526" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.3">
@@ -8504,7 +8501,7 @@
         <v>527</v>
       </c>
       <c r="C527" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.3">
@@ -8515,7 +8512,7 @@
         <v>528</v>
       </c>
       <c r="C528" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.3">
@@ -8526,7 +8523,7 @@
         <v>529</v>
       </c>
       <c r="C529" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.3">
@@ -8537,7 +8534,7 @@
         <v>530</v>
       </c>
       <c r="C530" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.3">
@@ -8548,7 +8545,7 @@
         <v>531</v>
       </c>
       <c r="C531" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.3">
@@ -8559,7 +8556,7 @@
         <v>532</v>
       </c>
       <c r="C532" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.3">
@@ -8570,7 +8567,7 @@
         <v>533</v>
       </c>
       <c r="C533" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.3">
@@ -8581,7 +8578,7 @@
         <v>534</v>
       </c>
       <c r="C534" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.3">
@@ -8592,7 +8589,7 @@
         <v>535</v>
       </c>
       <c r="C535" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.3">
@@ -8603,7 +8600,7 @@
         <v>536</v>
       </c>
       <c r="C536" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.3">
@@ -8614,7 +8611,7 @@
         <v>537</v>
       </c>
       <c r="C537" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.3">
@@ -8625,7 +8622,7 @@
         <v>538</v>
       </c>
       <c r="C538" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.3">
@@ -8636,7 +8633,7 @@
         <v>539</v>
       </c>
       <c r="C539" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.3">
@@ -8647,7 +8644,7 @@
         <v>540</v>
       </c>
       <c r="C540" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.3">
@@ -8658,7 +8655,7 @@
         <v>541</v>
       </c>
       <c r="C541" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.3">
@@ -8669,7 +8666,7 @@
         <v>542</v>
       </c>
       <c r="C542" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.3">
@@ -8680,7 +8677,7 @@
         <v>543</v>
       </c>
       <c r="C543" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.3">
@@ -8691,7 +8688,7 @@
         <v>544</v>
       </c>
       <c r="C544" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.3">
@@ -8702,7 +8699,7 @@
         <v>545</v>
       </c>
       <c r="C545" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.3">
@@ -8713,7 +8710,7 @@
         <v>546</v>
       </c>
       <c r="C546" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.3">
@@ -8724,7 +8721,7 @@
         <v>547</v>
       </c>
       <c r="C547" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.3">
@@ -8735,7 +8732,7 @@
         <v>548</v>
       </c>
       <c r="C548" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.3">
@@ -8746,7 +8743,7 @@
         <v>549</v>
       </c>
       <c r="C549" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.3">
@@ -8757,7 +8754,7 @@
         <v>550</v>
       </c>
       <c r="C550" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.3">
@@ -8768,7 +8765,7 @@
         <v>551</v>
       </c>
       <c r="C551" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.3">
@@ -8779,7 +8776,7 @@
         <v>552</v>
       </c>
       <c r="C552" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.3">
@@ -8790,7 +8787,7 @@
         <v>553</v>
       </c>
       <c r="C553" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.3">
@@ -8801,7 +8798,7 @@
         <v>554</v>
       </c>
       <c r="C554" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.3">
@@ -8812,7 +8809,7 @@
         <v>555</v>
       </c>
       <c r="C555" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.3">
@@ -8823,7 +8820,7 @@
         <v>556</v>
       </c>
       <c r="C556" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.3">
@@ -8834,7 +8831,7 @@
         <v>557</v>
       </c>
       <c r="C557" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.3">
@@ -8845,7 +8842,7 @@
         <v>558</v>
       </c>
       <c r="C558" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.3">
@@ -8856,7 +8853,7 @@
         <v>559</v>
       </c>
       <c r="C559" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.3">
@@ -8867,7 +8864,7 @@
         <v>560</v>
       </c>
       <c r="C560" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.3">
@@ -8878,7 +8875,7 @@
         <v>561</v>
       </c>
       <c r="C561" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.3">
@@ -8889,7 +8886,7 @@
         <v>562</v>
       </c>
       <c r="C562" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.3">
@@ -8900,7 +8897,7 @@
         <v>563</v>
       </c>
       <c r="C563" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.3">
@@ -8911,7 +8908,7 @@
         <v>564</v>
       </c>
       <c r="C564" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.3">
@@ -8922,7 +8919,7 @@
         <v>565</v>
       </c>
       <c r="C565" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.3">
@@ -8933,7 +8930,7 @@
         <v>566</v>
       </c>
       <c r="C566" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.3">
@@ -8944,7 +8941,7 @@
         <v>567</v>
       </c>
       <c r="C567" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.3">
@@ -8955,7 +8952,7 @@
         <v>568</v>
       </c>
       <c r="C568" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.3">
@@ -8966,7 +8963,7 @@
         <v>569</v>
       </c>
       <c r="C569" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.3">
@@ -8977,7 +8974,7 @@
         <v>570</v>
       </c>
       <c r="C570" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.3">
@@ -8988,7 +8985,7 @@
         <v>571</v>
       </c>
       <c r="C571" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.3">
@@ -8999,7 +8996,7 @@
         <v>572</v>
       </c>
       <c r="C572" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.3">
@@ -9010,7 +9007,7 @@
         <v>573</v>
       </c>
       <c r="C573" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.3">
@@ -9021,7 +9018,7 @@
         <v>574</v>
       </c>
       <c r="C574" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.3">
@@ -9032,7 +9029,7 @@
         <v>575</v>
       </c>
       <c r="C575" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.3">
@@ -9043,7 +9040,7 @@
         <v>576</v>
       </c>
       <c r="C576" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.3">
@@ -9054,7 +9051,7 @@
         <v>577</v>
       </c>
       <c r="C577" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.3">
@@ -9065,7 +9062,7 @@
         <v>578</v>
       </c>
       <c r="C578" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.3">
@@ -9076,7 +9073,7 @@
         <v>579</v>
       </c>
       <c r="C579" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.3">
@@ -9087,7 +9084,7 @@
         <v>580</v>
       </c>
       <c r="C580" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.3">
@@ -9098,7 +9095,7 @@
         <v>581</v>
       </c>
       <c r="C581" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.3">
@@ -9109,7 +9106,7 @@
         <v>582</v>
       </c>
       <c r="C582" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.3">
@@ -9120,7 +9117,7 @@
         <v>583</v>
       </c>
       <c r="C583" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="584" spans="1:3" x14ac:dyDescent="0.3">
@@ -9131,7 +9128,7 @@
         <v>584</v>
       </c>
       <c r="C584" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.3">
@@ -9142,7 +9139,7 @@
         <v>585</v>
       </c>
       <c r="C585" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="586" spans="1:3" x14ac:dyDescent="0.3">
@@ -9153,7 +9150,7 @@
         <v>586</v>
       </c>
       <c r="C586" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="587" spans="1:3" x14ac:dyDescent="0.3">
@@ -9164,7 +9161,7 @@
         <v>587</v>
       </c>
       <c r="C587" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="588" spans="1:3" x14ac:dyDescent="0.3">
@@ -9175,7 +9172,7 @@
         <v>588</v>
       </c>
       <c r="C588" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="589" spans="1:3" x14ac:dyDescent="0.3">
@@ -9186,7 +9183,7 @@
         <v>589</v>
       </c>
       <c r="C589" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="590" spans="1:3" x14ac:dyDescent="0.3">
@@ -9197,7 +9194,7 @@
         <v>590</v>
       </c>
       <c r="C590" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="591" spans="1:3" x14ac:dyDescent="0.3">
@@ -9208,7 +9205,7 @@
         <v>591</v>
       </c>
       <c r="C591" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="592" spans="1:3" x14ac:dyDescent="0.3">
@@ -9219,7 +9216,7 @@
         <v>592</v>
       </c>
       <c r="C592" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="593" spans="1:3" x14ac:dyDescent="0.3">
@@ -9230,7 +9227,7 @@
         <v>593</v>
       </c>
       <c r="C593" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="594" spans="1:3" x14ac:dyDescent="0.3">
@@ -9241,7 +9238,7 @@
         <v>594</v>
       </c>
       <c r="C594" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.3">
@@ -9252,7 +9249,7 @@
         <v>595</v>
       </c>
       <c r="C595" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.3">
@@ -9263,7 +9260,7 @@
         <v>596</v>
       </c>
       <c r="C596" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.3">
@@ -9274,7 +9271,7 @@
         <v>597</v>
       </c>
       <c r="C597" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.3">
@@ -9285,7 +9282,7 @@
         <v>598</v>
       </c>
       <c r="C598" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.3">
@@ -9296,7 +9293,7 @@
         <v>599</v>
       </c>
       <c r="C599" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.3">
@@ -9307,7 +9304,7 @@
         <v>600</v>
       </c>
       <c r="C600" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.3">
@@ -9318,7 +9315,7 @@
         <v>601</v>
       </c>
       <c r="C601" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="602" spans="1:3" x14ac:dyDescent="0.3">
@@ -9329,7 +9326,7 @@
         <v>602</v>
       </c>
       <c r="C602" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.3">
@@ -9340,7 +9337,7 @@
         <v>603</v>
       </c>
       <c r="C603" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="604" spans="1:3" x14ac:dyDescent="0.3">
@@ -9351,7 +9348,7 @@
         <v>604</v>
       </c>
       <c r="C604" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="605" spans="1:3" x14ac:dyDescent="0.3">
@@ -9362,7 +9359,7 @@
         <v>605</v>
       </c>
       <c r="C605" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="606" spans="1:3" x14ac:dyDescent="0.3">
@@ -9373,7 +9370,7 @@
         <v>606</v>
       </c>
       <c r="C606" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.3">
@@ -9384,7 +9381,7 @@
         <v>607</v>
       </c>
       <c r="C607" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.3">
@@ -9395,7 +9392,7 @@
         <v>608</v>
       </c>
       <c r="C608" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.3">
@@ -9406,7 +9403,7 @@
         <v>609</v>
       </c>
       <c r="C609" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.3">
@@ -9417,7 +9414,7 @@
         <v>610</v>
       </c>
       <c r="C610" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="611" spans="1:3" x14ac:dyDescent="0.3">
@@ -9428,7 +9425,7 @@
         <v>611</v>
       </c>
       <c r="C611" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="612" spans="1:3" x14ac:dyDescent="0.3">
@@ -9439,7 +9436,7 @@
         <v>612</v>
       </c>
       <c r="C612" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="613" spans="1:3" x14ac:dyDescent="0.3">
@@ -9450,7 +9447,7 @@
         <v>613</v>
       </c>
       <c r="C613" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="614" spans="1:3" x14ac:dyDescent="0.3">
@@ -9461,7 +9458,7 @@
         <v>614</v>
       </c>
       <c r="C614" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="615" spans="1:3" x14ac:dyDescent="0.3">
@@ -9472,7 +9469,7 @@
         <v>615</v>
       </c>
       <c r="C615" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="616" spans="1:3" x14ac:dyDescent="0.3">
@@ -9483,7 +9480,7 @@
         <v>616</v>
       </c>
       <c r="C616" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="617" spans="1:3" x14ac:dyDescent="0.3">
@@ -9494,7 +9491,7 @@
         <v>617</v>
       </c>
       <c r="C617" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.3">
@@ -9505,7 +9502,7 @@
         <v>618</v>
       </c>
       <c r="C618" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.3">
@@ -9516,7 +9513,7 @@
         <v>619</v>
       </c>
       <c r="C619" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="620" spans="1:3" x14ac:dyDescent="0.3">
@@ -9527,7 +9524,7 @@
         <v>620</v>
       </c>
       <c r="C620" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="621" spans="1:3" x14ac:dyDescent="0.3">
@@ -9538,7 +9535,7 @@
         <v>621</v>
       </c>
       <c r="C621" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.3">
@@ -9549,7 +9546,7 @@
         <v>622</v>
       </c>
       <c r="C622" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.3">
@@ -9560,7 +9557,7 @@
         <v>623</v>
       </c>
       <c r="C623" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.3">
@@ -9571,7 +9568,7 @@
         <v>624</v>
       </c>
       <c r="C624" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
@@ -9582,7 +9579,7 @@
         <v>625</v>
       </c>
       <c r="C625" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
@@ -9593,7 +9590,7 @@
         <v>626</v>
       </c>
       <c r="C626" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.3">
@@ -9604,7 +9601,7 @@
         <v>627</v>
       </c>
       <c r="C627" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.3">
@@ -9615,7 +9612,7 @@
         <v>628</v>
       </c>
       <c r="C628" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.3">
@@ -9626,7 +9623,7 @@
         <v>629</v>
       </c>
       <c r="C629" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.3">
@@ -9637,7 +9634,7 @@
         <v>630</v>
       </c>
       <c r="C630" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.3">
@@ -9648,7 +9645,7 @@
         <v>631</v>
       </c>
       <c r="C631" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
@@ -9659,7 +9656,7 @@
         <v>632</v>
       </c>
       <c r="C632" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.3">
@@ -9670,7 +9667,7 @@
         <v>633</v>
       </c>
       <c r="C633" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.3">
@@ -9681,7 +9678,7 @@
         <v>634</v>
       </c>
       <c r="C634" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.3">
@@ -9692,7 +9689,7 @@
         <v>635</v>
       </c>
       <c r="C635" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.3">
@@ -9703,7 +9700,7 @@
         <v>636</v>
       </c>
       <c r="C636" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.3">
@@ -9714,7 +9711,7 @@
         <v>637</v>
       </c>
       <c r="C637" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.3">
@@ -9725,7 +9722,7 @@
         <v>638</v>
       </c>
       <c r="C638" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.3">
@@ -9736,7 +9733,7 @@
         <v>639</v>
       </c>
       <c r="C639" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.3">
@@ -9747,7 +9744,7 @@
         <v>640</v>
       </c>
       <c r="C640" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="641" spans="1:3" x14ac:dyDescent="0.3">
@@ -9758,7 +9755,7 @@
         <v>641</v>
       </c>
       <c r="C641" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="642" spans="1:3" x14ac:dyDescent="0.3">
@@ -9769,7 +9766,7 @@
         <v>642</v>
       </c>
       <c r="C642" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="643" spans="1:3" x14ac:dyDescent="0.3">
@@ -9780,7 +9777,7 @@
         <v>643</v>
       </c>
       <c r="C643" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="644" spans="1:3" x14ac:dyDescent="0.3">
@@ -9791,7 +9788,7 @@
         <v>644</v>
       </c>
       <c r="C644" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="645" spans="1:3" x14ac:dyDescent="0.3">
@@ -9802,7 +9799,7 @@
         <v>645</v>
       </c>
       <c r="C645" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.3">
@@ -9813,7 +9810,7 @@
         <v>646</v>
       </c>
       <c r="C646" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="647" spans="1:3" x14ac:dyDescent="0.3">
@@ -9824,7 +9821,7 @@
         <v>647</v>
       </c>
       <c r="C647" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="648" spans="1:3" x14ac:dyDescent="0.3">
@@ -9835,7 +9832,7 @@
         <v>648</v>
       </c>
       <c r="C648" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.3">
@@ -9846,7 +9843,7 @@
         <v>649</v>
       </c>
       <c r="C649" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="650" spans="1:3" x14ac:dyDescent="0.3">
@@ -9857,7 +9854,7 @@
         <v>650</v>
       </c>
       <c r="C650" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.3">
@@ -9868,7 +9865,7 @@
         <v>651</v>
       </c>
       <c r="C651" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.3">
@@ -9879,7 +9876,7 @@
         <v>652</v>
       </c>
       <c r="C652" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.3">
@@ -9890,7 +9887,7 @@
         <v>653</v>
       </c>
       <c r="C653" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.3">
@@ -9901,7 +9898,7 @@
         <v>654</v>
       </c>
       <c r="C654" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="655" spans="1:3" x14ac:dyDescent="0.3">
@@ -9912,7 +9909,7 @@
         <v>655</v>
       </c>
       <c r="C655" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.3">
@@ -9923,7 +9920,7 @@
         <v>656</v>
       </c>
       <c r="C656" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="657" spans="1:3" x14ac:dyDescent="0.3">
@@ -9934,7 +9931,7 @@
         <v>657</v>
       </c>
       <c r="C657" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.3">
@@ -9945,7 +9942,7 @@
         <v>658</v>
       </c>
       <c r="C658" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="659" spans="1:3" x14ac:dyDescent="0.3">
@@ -9956,7 +9953,7 @@
         <v>659</v>
       </c>
       <c r="C659" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="660" spans="1:3" x14ac:dyDescent="0.3">
@@ -9967,7 +9964,7 @@
         <v>660</v>
       </c>
       <c r="C660" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="661" spans="1:3" x14ac:dyDescent="0.3">
@@ -9978,7 +9975,7 @@
         <v>661</v>
       </c>
       <c r="C661" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.3">
@@ -9989,7 +9986,7 @@
         <v>662</v>
       </c>
       <c r="C662" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="663" spans="1:3" x14ac:dyDescent="0.3">
@@ -10000,7 +9997,7 @@
         <v>663</v>
       </c>
       <c r="C663" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="664" spans="1:3" x14ac:dyDescent="0.3">
@@ -10011,7 +10008,7 @@
         <v>664</v>
       </c>
       <c r="C664" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.3">
@@ -10022,7 +10019,7 @@
         <v>665</v>
       </c>
       <c r="C665" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.3">
@@ -10033,7 +10030,7 @@
         <v>666</v>
       </c>
       <c r="C666" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.3">
@@ -10044,7 +10041,7 @@
         <v>667</v>
       </c>
       <c r="C667" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="668" spans="1:3" x14ac:dyDescent="0.3">
@@ -10055,7 +10052,7 @@
         <v>668</v>
       </c>
       <c r="C668" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.3">
@@ -10066,7 +10063,7 @@
         <v>669</v>
       </c>
       <c r="C669" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.3">
@@ -10077,7 +10074,7 @@
         <v>670</v>
       </c>
       <c r="C670" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="671" spans="1:3" x14ac:dyDescent="0.3">
@@ -10088,7 +10085,7 @@
         <v>671</v>
       </c>
       <c r="C671" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="672" spans="1:3" x14ac:dyDescent="0.3">
@@ -10099,7 +10096,7 @@
         <v>672</v>
       </c>
       <c r="C672" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="673" spans="1:3" x14ac:dyDescent="0.3">
@@ -10110,7 +10107,7 @@
         <v>673</v>
       </c>
       <c r="C673" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.3">
@@ -10121,7 +10118,7 @@
         <v>674</v>
       </c>
       <c r="C674" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="675" spans="1:3" x14ac:dyDescent="0.3">
@@ -10132,7 +10129,7 @@
         <v>675</v>
       </c>
       <c r="C675" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="676" spans="1:3" x14ac:dyDescent="0.3">
@@ -10143,7 +10140,7 @@
         <v>676</v>
       </c>
       <c r="C676" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="677" spans="1:3" x14ac:dyDescent="0.3">
@@ -10154,7 +10151,7 @@
         <v>677</v>
       </c>
       <c r="C677" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.3">
@@ -10165,7 +10162,7 @@
         <v>678</v>
       </c>
       <c r="C678" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="679" spans="1:3" x14ac:dyDescent="0.3">
@@ -10176,7 +10173,7 @@
         <v>679</v>
       </c>
       <c r="C679" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="680" spans="1:3" x14ac:dyDescent="0.3">
@@ -10187,7 +10184,7 @@
         <v>680</v>
       </c>
       <c r="C680" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="681" spans="1:3" x14ac:dyDescent="0.3">
@@ -10198,7 +10195,7 @@
         <v>681</v>
       </c>
       <c r="C681" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="682" spans="1:3" x14ac:dyDescent="0.3">
@@ -10209,7 +10206,7 @@
         <v>682</v>
       </c>
       <c r="C682" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="683" spans="1:3" x14ac:dyDescent="0.3">
@@ -10220,7 +10217,7 @@
         <v>683</v>
       </c>
       <c r="C683" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="684" spans="1:3" x14ac:dyDescent="0.3">
@@ -10231,7 +10228,7 @@
         <v>684</v>
       </c>
       <c r="C684" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="685" spans="1:3" x14ac:dyDescent="0.3">
@@ -10242,7 +10239,7 @@
         <v>685</v>
       </c>
       <c r="C685" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="686" spans="1:3" x14ac:dyDescent="0.3">
@@ -10253,7 +10250,7 @@
         <v>686</v>
       </c>
       <c r="C686" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="687" spans="1:3" x14ac:dyDescent="0.3">
@@ -10264,7 +10261,7 @@
         <v>687</v>
       </c>
       <c r="C687" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="688" spans="1:3" x14ac:dyDescent="0.3">
@@ -10275,7 +10272,7 @@
         <v>688</v>
       </c>
       <c r="C688" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.3">
@@ -10286,7 +10283,7 @@
         <v>689</v>
       </c>
       <c r="C689" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="690" spans="1:3" x14ac:dyDescent="0.3">
@@ -10297,7 +10294,7 @@
         <v>690</v>
       </c>
       <c r="C690" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.3">
@@ -10308,7 +10305,7 @@
         <v>691</v>
       </c>
       <c r="C691" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="692" spans="1:3" x14ac:dyDescent="0.3">
@@ -10319,7 +10316,7 @@
         <v>692</v>
       </c>
       <c r="C692" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="693" spans="1:3" x14ac:dyDescent="0.3">
@@ -10330,7 +10327,7 @@
         <v>693</v>
       </c>
       <c r="C693" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="694" spans="1:3" x14ac:dyDescent="0.3">
@@ -10341,7 +10338,7 @@
         <v>694</v>
       </c>
       <c r="C694" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="695" spans="1:3" x14ac:dyDescent="0.3">
@@ -10352,7 +10349,7 @@
         <v>695</v>
       </c>
       <c r="C695" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="696" spans="1:3" x14ac:dyDescent="0.3">
@@ -10363,7 +10360,7 @@
         <v>696</v>
       </c>
       <c r="C696" t="s">
-        <v>325</v>
+        <v>697</v>
       </c>
     </row>
     <row r="697" spans="1:3" x14ac:dyDescent="0.3">
@@ -10371,10 +10368,10 @@
         <v>696</v>
       </c>
       <c r="B697" t="s">
+        <v>698</v>
+      </c>
+      <c r="C697" t="s">
         <v>697</v>
-      </c>
-      <c r="C697" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="698" spans="1:3" x14ac:dyDescent="0.3">
@@ -10385,7 +10382,7 @@
         <v>699</v>
       </c>
       <c r="C698" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="699" spans="1:3" x14ac:dyDescent="0.3">
@@ -10396,7 +10393,7 @@
         <v>700</v>
       </c>
       <c r="C699" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="700" spans="1:3" x14ac:dyDescent="0.3">
@@ -10407,7 +10404,7 @@
         <v>701</v>
       </c>
       <c r="C700" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="701" spans="1:3" x14ac:dyDescent="0.3">
@@ -10418,7 +10415,7 @@
         <v>702</v>
       </c>
       <c r="C701" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="702" spans="1:3" x14ac:dyDescent="0.3">
@@ -10429,7 +10426,7 @@
         <v>703</v>
       </c>
       <c r="C702" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="703" spans="1:3" x14ac:dyDescent="0.3">
@@ -10440,7 +10437,7 @@
         <v>704</v>
       </c>
       <c r="C703" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="704" spans="1:3" x14ac:dyDescent="0.3">
@@ -10451,7 +10448,7 @@
         <v>705</v>
       </c>
       <c r="C704" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="705" spans="1:3" x14ac:dyDescent="0.3">
@@ -10462,7 +10459,7 @@
         <v>706</v>
       </c>
       <c r="C705" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="706" spans="1:3" x14ac:dyDescent="0.3">
@@ -10473,7 +10470,7 @@
         <v>707</v>
       </c>
       <c r="C706" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="707" spans="1:3" x14ac:dyDescent="0.3">
@@ -10484,7 +10481,7 @@
         <v>708</v>
       </c>
       <c r="C707" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="708" spans="1:3" x14ac:dyDescent="0.3">
@@ -10495,7 +10492,7 @@
         <v>709</v>
       </c>
       <c r="C708" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="709" spans="1:3" x14ac:dyDescent="0.3">
@@ -10506,7 +10503,7 @@
         <v>710</v>
       </c>
       <c r="C709" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="710" spans="1:3" x14ac:dyDescent="0.3">
@@ -10517,7 +10514,7 @@
         <v>711</v>
       </c>
       <c r="C710" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="711" spans="1:3" x14ac:dyDescent="0.3">
@@ -10528,7 +10525,7 @@
         <v>712</v>
       </c>
       <c r="C711" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="712" spans="1:3" x14ac:dyDescent="0.3">
@@ -10539,7 +10536,7 @@
         <v>713</v>
       </c>
       <c r="C712" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="713" spans="1:3" x14ac:dyDescent="0.3">
@@ -10550,7 +10547,7 @@
         <v>714</v>
       </c>
       <c r="C713" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="714" spans="1:3" x14ac:dyDescent="0.3">
@@ -10561,7 +10558,7 @@
         <v>715</v>
       </c>
       <c r="C714" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="715" spans="1:3" x14ac:dyDescent="0.3">
@@ -10572,7 +10569,7 @@
         <v>716</v>
       </c>
       <c r="C715" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="716" spans="1:3" x14ac:dyDescent="0.3">
@@ -10583,7 +10580,7 @@
         <v>717</v>
       </c>
       <c r="C716" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="717" spans="1:3" x14ac:dyDescent="0.3">
@@ -10594,7 +10591,7 @@
         <v>718</v>
       </c>
       <c r="C717" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="718" spans="1:3" x14ac:dyDescent="0.3">
@@ -10605,7 +10602,7 @@
         <v>719</v>
       </c>
       <c r="C718" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="719" spans="1:3" x14ac:dyDescent="0.3">
@@ -10616,7 +10613,7 @@
         <v>720</v>
       </c>
       <c r="C719" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="720" spans="1:3" x14ac:dyDescent="0.3">
@@ -10627,7 +10624,7 @@
         <v>721</v>
       </c>
       <c r="C720" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="721" spans="1:3" x14ac:dyDescent="0.3">
@@ -10638,7 +10635,7 @@
         <v>722</v>
       </c>
       <c r="C721" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="722" spans="1:3" x14ac:dyDescent="0.3">
@@ -10649,7 +10646,7 @@
         <v>723</v>
       </c>
       <c r="C722" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="723" spans="1:3" x14ac:dyDescent="0.3">
@@ -10660,7 +10657,7 @@
         <v>724</v>
       </c>
       <c r="C723" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="724" spans="1:3" x14ac:dyDescent="0.3">
@@ -10671,7 +10668,7 @@
         <v>725</v>
       </c>
       <c r="C724" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="725" spans="1:3" x14ac:dyDescent="0.3">
@@ -10682,7 +10679,7 @@
         <v>726</v>
       </c>
       <c r="C725" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="726" spans="1:3" x14ac:dyDescent="0.3">
@@ -10693,7 +10690,7 @@
         <v>727</v>
       </c>
       <c r="C726" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="727" spans="1:3" x14ac:dyDescent="0.3">
@@ -10704,7 +10701,7 @@
         <v>728</v>
       </c>
       <c r="C727" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="728" spans="1:3" x14ac:dyDescent="0.3">
@@ -10715,7 +10712,7 @@
         <v>729</v>
       </c>
       <c r="C728" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="729" spans="1:3" x14ac:dyDescent="0.3">
@@ -10726,7 +10723,7 @@
         <v>730</v>
       </c>
       <c r="C729" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="730" spans="1:3" x14ac:dyDescent="0.3">
@@ -10737,7 +10734,7 @@
         <v>731</v>
       </c>
       <c r="C730" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="731" spans="1:3" x14ac:dyDescent="0.3">
@@ -10748,7 +10745,7 @@
         <v>732</v>
       </c>
       <c r="C731" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="732" spans="1:3" x14ac:dyDescent="0.3">
@@ -10759,7 +10756,7 @@
         <v>733</v>
       </c>
       <c r="C732" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="733" spans="1:3" x14ac:dyDescent="0.3">
@@ -10770,7 +10767,7 @@
         <v>734</v>
       </c>
       <c r="C733" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="734" spans="1:3" x14ac:dyDescent="0.3">
@@ -10781,7 +10778,7 @@
         <v>735</v>
       </c>
       <c r="C734" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="735" spans="1:3" x14ac:dyDescent="0.3">
@@ -10792,7 +10789,7 @@
         <v>736</v>
       </c>
       <c r="C735" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="736" spans="1:3" x14ac:dyDescent="0.3">
@@ -10803,7 +10800,7 @@
         <v>737</v>
       </c>
       <c r="C736" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="737" spans="1:3" x14ac:dyDescent="0.3">
@@ -10814,7 +10811,7 @@
         <v>738</v>
       </c>
       <c r="C737" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.3">
@@ -10825,7 +10822,7 @@
         <v>739</v>
       </c>
       <c r="C738" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="739" spans="1:3" x14ac:dyDescent="0.3">
@@ -10836,7 +10833,7 @@
         <v>740</v>
       </c>
       <c r="C739" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="740" spans="1:3" x14ac:dyDescent="0.3">
@@ -10847,7 +10844,7 @@
         <v>741</v>
       </c>
       <c r="C740" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="741" spans="1:3" x14ac:dyDescent="0.3">
@@ -10858,7 +10855,7 @@
         <v>742</v>
       </c>
       <c r="C741" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="742" spans="1:3" x14ac:dyDescent="0.3">
@@ -10869,7 +10866,7 @@
         <v>743</v>
       </c>
       <c r="C742" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="743" spans="1:3" x14ac:dyDescent="0.3">
@@ -10880,7 +10877,7 @@
         <v>744</v>
       </c>
       <c r="C743" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="744" spans="1:3" x14ac:dyDescent="0.3">
@@ -10891,7 +10888,7 @@
         <v>745</v>
       </c>
       <c r="C744" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="745" spans="1:3" x14ac:dyDescent="0.3">
@@ -10902,7 +10899,7 @@
         <v>746</v>
       </c>
       <c r="C745" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="746" spans="1:3" x14ac:dyDescent="0.3">
@@ -10913,7 +10910,7 @@
         <v>747</v>
       </c>
       <c r="C746" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="747" spans="1:3" x14ac:dyDescent="0.3">
@@ -10924,7 +10921,7 @@
         <v>748</v>
       </c>
       <c r="C747" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="748" spans="1:3" x14ac:dyDescent="0.3">
@@ -10935,7 +10932,7 @@
         <v>749</v>
       </c>
       <c r="C748" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="749" spans="1:3" x14ac:dyDescent="0.3">
@@ -10946,7 +10943,7 @@
         <v>750</v>
       </c>
       <c r="C749" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="750" spans="1:3" x14ac:dyDescent="0.3">
@@ -10957,7 +10954,7 @@
         <v>751</v>
       </c>
       <c r="C750" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="751" spans="1:3" x14ac:dyDescent="0.3">
@@ -10968,7 +10965,7 @@
         <v>752</v>
       </c>
       <c r="C751" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="752" spans="1:3" x14ac:dyDescent="0.3">
@@ -10979,7 +10976,7 @@
         <v>753</v>
       </c>
       <c r="C752" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="753" spans="1:3" x14ac:dyDescent="0.3">
@@ -10990,7 +10987,7 @@
         <v>754</v>
       </c>
       <c r="C753" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="754" spans="1:3" x14ac:dyDescent="0.3">
@@ -11001,7 +10998,7 @@
         <v>755</v>
       </c>
       <c r="C754" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.3">
@@ -11012,7 +11009,7 @@
         <v>756</v>
       </c>
       <c r="C755" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.3">
@@ -11023,7 +11020,7 @@
         <v>757</v>
       </c>
       <c r="C756" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="757" spans="1:3" x14ac:dyDescent="0.3">
@@ -11034,7 +11031,7 @@
         <v>758</v>
       </c>
       <c r="C757" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="758" spans="1:3" x14ac:dyDescent="0.3">
@@ -11045,7 +11042,7 @@
         <v>759</v>
       </c>
       <c r="C758" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="759" spans="1:3" x14ac:dyDescent="0.3">
@@ -11056,7 +11053,7 @@
         <v>760</v>
       </c>
       <c r="C759" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.3">
@@ -11067,7 +11064,7 @@
         <v>761</v>
       </c>
       <c r="C760" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.3">
@@ -11078,7 +11075,7 @@
         <v>762</v>
       </c>
       <c r="C761" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.3">
@@ -11089,7 +11086,7 @@
         <v>763</v>
       </c>
       <c r="C762" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.3">
@@ -11100,7 +11097,7 @@
         <v>764</v>
       </c>
       <c r="C763" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.3">
@@ -11111,7 +11108,7 @@
         <v>765</v>
       </c>
       <c r="C764" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.3">
@@ -11122,7 +11119,7 @@
         <v>766</v>
       </c>
       <c r="C765" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.3">
@@ -11133,7 +11130,7 @@
         <v>767</v>
       </c>
       <c r="C766" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.3">
@@ -11144,7 +11141,7 @@
         <v>768</v>
       </c>
       <c r="C767" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.3">
@@ -11155,7 +11152,7 @@
         <v>769</v>
       </c>
       <c r="C768" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.3">
@@ -11166,7 +11163,7 @@
         <v>770</v>
       </c>
       <c r="C769" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.3">
@@ -11177,7 +11174,7 @@
         <v>771</v>
       </c>
       <c r="C770" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="771" spans="1:3" x14ac:dyDescent="0.3">
@@ -11188,7 +11185,7 @@
         <v>772</v>
       </c>
       <c r="C771" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="772" spans="1:3" x14ac:dyDescent="0.3">
@@ -11199,7 +11196,7 @@
         <v>773</v>
       </c>
       <c r="C772" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="773" spans="1:3" x14ac:dyDescent="0.3">
@@ -11210,7 +11207,7 @@
         <v>774</v>
       </c>
       <c r="C773" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.3">
@@ -11221,7 +11218,7 @@
         <v>775</v>
       </c>
       <c r="C774" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="775" spans="1:3" x14ac:dyDescent="0.3">
@@ -11232,7 +11229,7 @@
         <v>776</v>
       </c>
       <c r="C775" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="776" spans="1:3" x14ac:dyDescent="0.3">
@@ -11243,7 +11240,7 @@
         <v>777</v>
       </c>
       <c r="C776" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.3">
@@ -11254,7 +11251,7 @@
         <v>778</v>
       </c>
       <c r="C777" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.3">
@@ -11262,10 +11259,10 @@
         <v>777</v>
       </c>
       <c r="B778" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C778" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>